<commit_message>
Cambios para el excel
</commit_message>
<xml_diff>
--- a/test/Tramites.xlsx
+++ b/test/Tramites.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>rodrigo</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>ALIMENTICIAS</t>
+  </si>
+  <si>
+    <t>calle 01</t>
   </si>
 </sst>
 </file>
@@ -436,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -450,7 +453,7 @@
     <col min="11" max="11" width="28.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -487,8 +490,20 @@
       <c r="L1" t="s">
         <v>14</v>
       </c>
+      <c r="M1">
+        <v>7980</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1">
+        <v>23</v>
+      </c>
+      <c r="P1">
+        <v>34</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -526,7 +541,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -564,7 +579,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>

</xml_diff>